<commit_message>
initial commits with new projects (derivation is not implemented)
</commit_message>
<xml_diff>
--- a/tests/data_minimal_case/files_info.xlsx
+++ b/tests/data_minimal_case/files_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/gcms_data_analysis/tests/data_minimal_case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Projects/gcms_data_analysis/tests/data_minimal_case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{10295F71-187C-406A-AF09-CB447617FFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7915FFD1-9C97-43D6-B46E-988CE4765A5A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8B946-8DC9-F444-841C-B05C2800C43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>samplename</t>
   </si>
   <si>
-    <t>replicate_number</t>
+    <t>replicatenumber</t>
   </si>
 </sst>
 </file>
@@ -108,6 +108,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,12 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,23 +441,22 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.41796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="36.83984375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="39.578125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="2"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="36.83203125" customWidth="1"/>
+    <col min="8" max="8" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,137 +482,137 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="b">
+      <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="b">
+      <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="b">
+      <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="b">
+      <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="b">
+      <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
   </sheetData>

</xml_diff>